<commit_message>
deck select on job error more obvious
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>正常</t>
   </si>
@@ -78,6 +78,10 @@
   </si>
   <si>
     <t>碎片不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>一套卡牌不能有两种职业卡牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -765,8 +769,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B14" totalsRowShown="0">
-  <autoFilter ref="A1:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B15" totalsRowShown="0">
+  <autoFilter ref="A1:B15"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Des"/>
@@ -1062,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1185,6 +1189,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>1004</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
close #77 eliminate the problem of wrong-encoding of dig form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>正常</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>一套卡牌不能有两种职业卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要等级到达{0}级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>体力不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>钻石不足</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -769,8 +781,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B15" totalsRowShown="0">
-  <autoFilter ref="A1:B15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B18" totalsRowShown="0">
+  <autoFilter ref="A1:B18"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Des"/>
@@ -1066,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1197,6 +1209,30 @@
         <v>17</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2001</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>3000</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
common card now can have 2 copies in the deck
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Error" sheetId="1" r:id="rId1"/>
@@ -61,14 +61,6 @@
     <t>Des</t>
   </si>
   <si>
-    <t>该卡牌已经入册</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>同种卡片只能入册1张</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>领导力不足</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -94,6 +86,14 @@
   </si>
   <si>
     <t>钻石不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>该卡牌只能入册2张</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>该卡牌只能入册1张</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1080,16 +1080,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>101</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>102</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>103</v>
       </c>
@@ -1153,39 +1153,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1001</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1002</v>
       </c>
@@ -1193,44 +1193,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1003</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1004</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2000</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2001</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3000</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #89 heroskill now has cD
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>正常</t>
   </si>
@@ -33,9 +33,6 @@
     <t>当前无法使用魔法卡片</t>
   </si>
   <si>
-    <t>魔法不足</t>
-  </si>
-  <si>
     <t>卡组已满</t>
   </si>
   <si>
@@ -61,14 +58,6 @@
     <t>Des</t>
   </si>
   <si>
-    <t>领导力不足</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>毅力不足</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>碎片不足</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -94,6 +83,22 @@
   </si>
   <si>
     <t>该卡牌只能入册1张</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英雄技能冷却中</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LP不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PP不足</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -781,8 +786,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B18" totalsRowShown="0">
-  <autoFilter ref="A1:B18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B19" totalsRowShown="0">
+  <autoFilter ref="A1:B19"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Des"/>
@@ -1078,7 +1083,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -1091,26 +1096,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1150,7 +1155,7 @@
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,7 +1163,7 @@
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,71 +1171,79 @@
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1000</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2000</v>
+        <v>1004</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>2001</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>3000</v>
       </c>
-      <c r="B18" t="s">
-        <v>18</v>
+      <c r="B19" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the scene chess move effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Error" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>需要等级到达{0}级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>体力不足</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -99,6 +95,10 @@
   </si>
   <si>
     <t>PP不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>不符合地图进入条件</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -774,6 +774,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -804,7 +872,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1086,15 +1154,15 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +1170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1110,7 +1178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1126,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1134,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>101</v>
       </c>
@@ -1142,7 +1210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>102</v>
       </c>
@@ -1150,55 +1218,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1000</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1001</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1002</v>
       </c>
@@ -1206,7 +1274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1003</v>
       </c>
@@ -1214,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1004</v>
       </c>
@@ -1222,28 +1290,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2000</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2001</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3000</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make SceneWarp relay on level to work
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>正常</t>
   </si>
@@ -98,7 +98,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>不符合地图进入条件</t>
+    <t>需要达到等级{0}才能进入</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先探索地图激活传送门</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -774,74 +778,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -854,8 +790,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B19" totalsRowShown="0">
-  <autoFilter ref="A1:B19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B20" totalsRowShown="0">
+  <autoFilter ref="A1:B20"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Des"/>
@@ -872,7 +808,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1151,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1308,9 +1244,17 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19">
+        <v>2002</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20">
         <v>3000</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
balance the deck cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>正常</t>
   </si>
@@ -104,12 +104,19 @@
   <si>
     <t>请先探索地图激活传送门</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>手牌满惩罚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌耗尽惩罚</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -790,8 +797,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B20" totalsRowShown="0">
-  <autoFilter ref="A1:B20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B22" totalsRowShown="0">
+  <autoFilter ref="A1:B22"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Des"/>
@@ -801,7 +808,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -876,6 +883,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -911,6 +935,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1087,14 +1128,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1188,73 +1230,89 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>1000</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>1001</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>2000</v>
+        <v>1003</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>2001</v>
+        <v>1004</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20">
+        <v>2001</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>2002</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22">
         <v>3000</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove expbottle, fix some small bugs
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>正常</t>
   </si>
@@ -58,10 +58,6 @@
     <t>Des</t>
   </si>
   <si>
-    <t>碎片不足</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>一套卡牌不能有两种职业卡牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -111,6 +107,14 @@
   </si>
   <si>
     <t>卡牌耗尽惩罚</t>
+  </si>
+  <si>
+    <t>没有可以分解的碎片</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级所需碎片不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -797,8 +801,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B22" totalsRowShown="0">
-  <autoFilter ref="A1:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B23" totalsRowShown="0">
+  <autoFilter ref="A1:B23"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Des"/>
@@ -1128,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1201,7 +1205,7 @@
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
@@ -1209,7 +1213,7 @@
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -1217,7 +1221,7 @@
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
@@ -1225,7 +1229,7 @@
         <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -1233,7 +1237,7 @@
         <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
@@ -1241,7 +1245,7 @@
         <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
@@ -1249,7 +1253,7 @@
         <v>1000</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
@@ -1257,7 +1261,7 @@
         <v>1001</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
@@ -1273,7 +1277,7 @@
         <v>1003</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
@@ -1281,39 +1285,47 @@
         <v>1004</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>2000</v>
+        <v>1005</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22">
+        <v>2002</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23">
         <v>3000</v>
       </c>
-      <c r="B22" t="s">
-        <v>14</v>
+      <c r="B23" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug on peiceform and changecard form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>正常</t>
   </si>
@@ -114,13 +114,17 @@
   </si>
   <si>
     <t>升级所需碎片不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源不足</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -801,11 +805,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B23" totalsRowShown="0">
-  <autoFilter ref="A1:B23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:B24" totalsRowShown="0">
+  <autoFilter ref="A1:B24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Des"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Des"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1131,11 +1135,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1328,6 +1332,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>3001</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
make the wheel form canbe configed
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>正常</t>
   </si>
@@ -118,6 +118,10 @@
   </si>
   <si>
     <t>资源不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>背包已满</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -805,8 +809,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:B24" totalsRowShown="0">
-  <autoFilter ref="A1:B24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:B25" totalsRowShown="0">
+  <autoFilter ref="A1:B25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Des"/>
@@ -1136,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1340,6 +1344,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>3002</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
merge the errortypes as a alias of Error.xlsx
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>正常</t>
   </si>
@@ -125,6 +125,87 @@
   </si>
   <si>
     <t>描述</t>
+  </si>
+  <si>
+    <t>别名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>CommonError</t>
+  </si>
+  <si>
+    <t>BattleNoUseCard</t>
+  </si>
+  <si>
+    <t>BattleNoUseSpellCard</t>
+  </si>
+  <si>
+    <t>BattleLackMp</t>
+  </si>
+  <si>
+    <t>BattleLackLp</t>
+  </si>
+  <si>
+    <t>BattleLackPp</t>
+  </si>
+  <si>
+    <t>BattleHeroSkillInCd</t>
+  </si>
+  <si>
+    <t>CardOutPunish</t>
+  </si>
+  <si>
+    <t>CardFullPunish</t>
+  </si>
+  <si>
+    <t>DeckCardTypeLimitLegend</t>
+  </si>
+  <si>
+    <t>DeckCardTypeLimit</t>
+  </si>
+  <si>
+    <t>DeckIsFull</t>
+  </si>
+  <si>
+    <t>CardExpNotEnough</t>
+  </si>
+  <si>
+    <t>CardExpNotEnough2</t>
+  </si>
+  <si>
+    <t>CardJobTwice</t>
+  </si>
+  <si>
+    <t>SceneLevelNeed</t>
+  </si>
+  <si>
+    <t>SceneAPNotEnough</t>
+  </si>
+  <si>
+    <t>SceneWarpNeedActive</t>
+  </si>
+  <si>
+    <t>BagNotEnoughDimond</t>
+  </si>
+  <si>
+    <t>BagNotEnoughResource</t>
+  </si>
+  <si>
+    <t>BagIsFull</t>
+  </si>
+  <si>
+    <t>BagNotEnoughItems</t>
   </si>
 </sst>
 </file>
@@ -879,10 +960,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B26" totalsRowShown="0">
-  <autoFilter ref="A1:B26"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:C26" totalsRowShown="0">
+  <autoFilter ref="A1:C26"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="错误id"/>
+    <tableColumn id="3" name="别名"/>
     <tableColumn id="2" name="描述"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1210,223 +1292,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>27</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>101</v>
       </c>
       <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>102</v>
       </c>
       <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>103</v>
       </c>
       <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>104</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>105</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>106</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>107</v>
       </c>
       <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>108</v>
       </c>
       <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1000</v>
       </c>
       <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1001</v>
       </c>
       <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1002</v>
       </c>
       <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>1003</v>
       </c>
       <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>1004</v>
       </c>
       <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>1005</v>
       </c>
       <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2000</v>
       </c>
       <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2001</v>
       </c>
       <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2002</v>
       </c>
       <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3000</v>
       </c>
       <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3001</v>
       </c>
       <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3002</v>
       </c>
       <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3003</v>
       </c>
       <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some error tip bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>正常</t>
   </si>
@@ -206,6 +206,30 @@
   </si>
   <si>
     <t>BagNotEnoughItems</t>
+  </si>
+  <si>
+    <t>完成任务【开始】开启转职</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>等级5开启转职</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>JobLevelLow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>JobQuestNotFin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BagNotEnoughGold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>金钱不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -960,8 +984,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:C26" totalsRowShown="0">
-  <autoFilter ref="A1:C26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:C29" totalsRowShown="0">
+  <autoFilter ref="A1:C29"/>
   <tableColumns count="3">
     <tableColumn id="1" name="错误id"/>
     <tableColumn id="3" name="别名"/>
@@ -1292,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1591,6 +1615,39 @@
         <v>26</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>3004</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>3005</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>3006</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
optimise the procedure of change job
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Error.xlsx
+++ b/ConfigData/Xlsx/Error.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A3B08D98-5F0B-4541-AB7B-85F0BFB0570A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error" sheetId="1" r:id="rId1"/>
@@ -212,14 +213,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>等级5开启转职</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>JobLevelLow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>JobQuestNotFin</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -229,13 +222,21 @@
   </si>
   <si>
     <t>金钱不足</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>JobNotInTown</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在城镇中才能切换职业</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -904,74 +905,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -984,12 +917,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:C29" totalsRowShown="0">
-  <autoFilter ref="A1:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:C29" totalsRowShown="0">
+  <autoFilter ref="A1:C29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="错误id"/>
-    <tableColumn id="3" name="别名"/>
-    <tableColumn id="2" name="描述"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="错误id"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="别名"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="描述"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1003,7 +936,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1315,11 +1248,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1620,10 +1553,10 @@
         <v>3004</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
@@ -1631,10 +1564,10 @@
         <v>3005</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -1642,7 +1575,7 @@
         <v>3006</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
         <v>55</v>

</xml_diff>